<commit_message>
whoita, 4et bagi kakieto
</commit_message>
<xml_diff>
--- a/dannie reweniy.xlsx
+++ b/dannie reweniy.xlsx
@@ -8,24 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neste\source\Repos\laba_6_antonov\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA498C1-05B4-4FB9-A913-AC7FF97DEFB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5884F53-5F00-4DD6-BD61-EB3EDB70E272}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3270" yWindow="855" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3450" yWindow="600" windowWidth="22740" windowHeight="13395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>время в сек</t>
   </si>
@@ -43,6 +49,48 @@
   </si>
   <si>
     <t>запись</t>
+  </si>
+  <si>
+    <t>улучшенная версия c бкастом</t>
+  </si>
+  <si>
+    <t>улучшенная в. С улуч.бкастом.</t>
+  </si>
+  <si>
+    <t>улуч.в.улуч.бкаст.</t>
+  </si>
+  <si>
+    <t>чтение</t>
+  </si>
+  <si>
+    <t>сумма</t>
+  </si>
+  <si>
+    <t>только счет</t>
+  </si>
+  <si>
+    <t>бкаст</t>
+  </si>
+  <si>
+    <t>кол. Проц</t>
+  </si>
+  <si>
+    <t>ч. На всех, без бкаста</t>
+  </si>
+  <si>
+    <t>общее</t>
+  </si>
+  <si>
+    <t>ср.вр.счета на процессе</t>
+  </si>
+  <si>
+    <t>просто счет круто да</t>
+  </si>
+  <si>
+    <t>только счет без учета отправок</t>
+  </si>
+  <si>
+    <t>сверху то что до оптимизаций было</t>
   </si>
 </sst>
 </file>
@@ -111,36 +159,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="ru-RU"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -148,8 +166,100 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$R$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>улуч.в.улуч.бкаст.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Лист1!$O$15:$O$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$U$15:$U$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1025.0466730000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>951.81876799999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>748.129639</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>730.68333399999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>604.92342399999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DCFD-4397-BB73-10A796F73EAA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$S$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>сумма</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -164,42 +274,48 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$B$2:$B$6</c:f>
+              <c:f>Лист1!$O$15:$O$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$C$2:$C$6</c:f>
+              <c:f>Лист1!$S$15:$S$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1157.6580120000001</c:v>
+                  <c:v>228</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1127.721526</c:v>
+                  <c:v>332</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>896.13710800000001</c:v>
+                  <c:v>175</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>809.24718800000005</c:v>
+                  <c:v>319</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>107</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -207,20 +323,20 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-EE46-4D2D-A065-1DE81C905CF8}"/>
+              <c16:uniqueId val="{00000002-DCFD-4397-BB73-10A796F73EAA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Лист1!$D$1</c:f>
+              <c:f>Лист1!$T$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>второй прогон</c:v>
+                  <c:v>только счет</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -239,42 +355,48 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Лист1!$B$2:$B$6</c:f>
+              <c:f>Лист1!$O$15:$O$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$D$2:$D$7</c:f>
+              <c:f>Лист1!$T$15:$T$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1117.290107</c:v>
+                  <c:v>797.04667300000006</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1058.2863709999999</c:v>
+                  <c:v>619.81876799999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>911.005448</c:v>
+                  <c:v>573.129639</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>821.39877100000001</c:v>
+                  <c:v>411.68333399999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>497.92342399999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -282,58 +404,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-EE46-4D2D-A065-1DE81C905CF8}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Лист1!$E$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>3 прогон, чтение на всех, без бкаста</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Лист1!$E$2:$E$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="1">
-                  <c:v>1081.583253</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>956.98339099999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>833.22255500000006</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-33C6-4F75-9284-8902AA1978D2}"/>
+              <c16:uniqueId val="{00000003-DCFD-4397-BB73-10A796F73EAA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -639,7 +710,933 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$U$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>общее</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Лист1!$O$14:$O$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$U$24:$U$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1431.5815720000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1238.7523229999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>774.31291699999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>633.665796</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>606.68988400000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>581.68473100000006</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8747-4667-B8B7-AC5C0BE1CB31}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$S$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>сумма</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Лист1!$O$14:$O$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$S$24:$S$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>123</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8747-4667-B8B7-AC5C0BE1CB31}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1507257696"/>
+        <c:axId val="1306509952"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1507257696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>кол проц</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1306509952"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1306509952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>время в сек</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.6522001205545511E-2"/>
+              <c:y val="0.33625134057361344"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1507257696"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$W$33</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>только счет без учета отправок</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Лист1!$O$34:$O$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$W$34:$W$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>755.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>610</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>627.20000000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>512.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>456</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>432</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-1D9E-4DE0-91EB-38666ADA83C9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$W$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Лист1!$O$34:$O$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$W$24:$W$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>768</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>440</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-1D9E-4DE0-91EB-38666ADA83C9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="234758719"/>
+        <c:axId val="41993135"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="234758719"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="41993135"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="41993135"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="234758719"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1195,20 +2192,1052 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>209551</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>171451</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1228,6 +3257,80 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>180976</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Диаграмма 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB9D4D3D-C106-4434-AE0D-8B9302E307EC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF84BBA3-F266-4A88-86BA-0CA441C59D3D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1499,20 +3602,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:I10"/>
+  <dimension ref="B1:W39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
-    <col min="5" max="5" width="36.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" customWidth="1"/>
+    <col min="20" max="20" width="11.85546875" customWidth="1"/>
+    <col min="21" max="21" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -1525,8 +3631,14 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>16</v>
       </c>
@@ -1536,8 +3648,11 @@
       <c r="D2">
         <v>1117.290107</v>
       </c>
+      <c r="G2">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>12</v>
       </c>
@@ -1550,8 +3665,11 @@
       <c r="E3">
         <v>1081.583253</v>
       </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>8</v>
       </c>
@@ -1564,8 +3682,14 @@
       <c r="E4">
         <v>956.98339099999998</v>
       </c>
+      <c r="F4">
+        <v>1150.7387719999999</v>
+      </c>
+      <c r="G4">
+        <v>8</v>
+      </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>4</v>
       </c>
@@ -1578,75 +3702,585 @@
       <c r="E5">
         <v>833.22255500000006</v>
       </c>
+      <c r="F5">
+        <v>840.79688099999998</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
         <v>4</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6">
         <v>4</v>
       </c>
-      <c r="G6" t="s">
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="P13" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>9</v>
+      </c>
+      <c r="R13" t="s">
+        <v>5</v>
+      </c>
+      <c r="S13" t="s">
+        <v>10</v>
+      </c>
+      <c r="T13" t="s">
+        <v>11</v>
+      </c>
+      <c r="U13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="O15">
+        <v>10</v>
+      </c>
+      <c r="P15">
+        <f>60+5*9</f>
+        <v>105</v>
+      </c>
+      <c r="Q15">
+        <v>61</v>
+      </c>
+      <c r="R15">
+        <v>62</v>
+      </c>
+      <c r="S15">
+        <f>P15+Q15+R15</f>
+        <v>228</v>
+      </c>
+      <c r="T15">
+        <f>U15-S15</f>
+        <v>797.04667300000006</v>
+      </c>
+      <c r="U15">
+        <v>1025.0466730000001</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="O16">
+        <v>8</v>
+      </c>
+      <c r="P16">
+        <f>30*8</f>
+        <v>240</v>
+      </c>
+      <c r="Q16">
+        <v>30</v>
+      </c>
+      <c r="R16">
+        <v>62</v>
+      </c>
+      <c r="S16">
+        <f>P16+Q16+R16</f>
+        <v>332</v>
+      </c>
+      <c r="T16">
+        <f>U16-S16</f>
+        <v>619.81876799999998</v>
+      </c>
+      <c r="U16">
+        <v>951.81876799999998</v>
+      </c>
+    </row>
+    <row r="17" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="O17">
+        <v>5</v>
+      </c>
+      <c r="P17">
+        <f>30+13*4</f>
+        <v>82</v>
+      </c>
+      <c r="Q17">
+        <v>30</v>
+      </c>
+      <c r="R17">
+        <v>63</v>
+      </c>
+      <c r="S17">
+        <f>P17+Q17+R17</f>
+        <v>175</v>
+      </c>
+      <c r="T17">
+        <f>U17-S17</f>
+        <v>573.129639</v>
+      </c>
+      <c r="U17">
+        <v>748.129639</v>
+      </c>
+    </row>
+    <row r="18" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="O18">
         <v>4</v>
       </c>
-      <c r="H6" t="s">
+      <c r="P18">
+        <f>30*4+20*4</f>
+        <v>200</v>
+      </c>
+      <c r="Q18">
+        <v>60</v>
+      </c>
+      <c r="R18">
+        <v>59</v>
+      </c>
+      <c r="S18">
+        <f>P18+Q18+R18</f>
+        <v>319</v>
+      </c>
+      <c r="T18">
+        <f>U18-S18</f>
+        <v>411.68333399999995</v>
+      </c>
+      <c r="U18">
+        <v>730.68333399999995</v>
+      </c>
+    </row>
+    <row r="19" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="O19">
+        <v>2</v>
+      </c>
+      <c r="P19">
+        <f>12</f>
+        <v>12</v>
+      </c>
+      <c r="Q19">
+        <v>30</v>
+      </c>
+      <c r="R19">
+        <v>65</v>
+      </c>
+      <c r="S19">
+        <f>P19+Q19+R19</f>
+        <v>107</v>
+      </c>
+      <c r="T19">
+        <f>U19-S19</f>
+        <v>497.92342399999995</v>
+      </c>
+      <c r="U19">
+        <v>604.92342399999995</v>
+      </c>
+    </row>
+    <row r="21" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="R21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="Q23" t="s">
+        <v>9</v>
+      </c>
+      <c r="R23" t="s">
+        <v>5</v>
+      </c>
+      <c r="S23" t="s">
+        <v>10</v>
+      </c>
+      <c r="T23" t="s">
+        <v>11</v>
+      </c>
+      <c r="U23" t="s">
+        <v>15</v>
+      </c>
+      <c r="V23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="O24">
+        <v>16</v>
+      </c>
+      <c r="Q24">
+        <v>65</v>
+      </c>
+      <c r="R24">
+        <v>63</v>
+      </c>
+      <c r="S24">
+        <f t="shared" ref="S24:S28" si="0">Q24+R24</f>
+        <v>128</v>
+      </c>
+      <c r="T24">
+        <f>U24-S24</f>
+        <v>1303.5815720000001</v>
+      </c>
+      <c r="U24">
+        <v>1431.5815720000001</v>
+      </c>
+      <c r="V24">
+        <v>3</v>
+      </c>
+      <c r="W24">
+        <f t="shared" ref="W24:W28" si="1">V24*O24*O24</f>
+        <v>768</v>
+      </c>
+    </row>
+    <row r="25" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="O25">
+        <v>10</v>
+      </c>
+      <c r="Q25">
+        <v>73</v>
+      </c>
+      <c r="R25">
+        <v>64</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="0"/>
+        <v>137</v>
+      </c>
+      <c r="T25">
+        <f t="shared" ref="T24:T25" si="2">U25-S25</f>
+        <v>1101.7523229999999</v>
+      </c>
+      <c r="U25">
+        <v>1238.7523229999999</v>
+      </c>
+      <c r="V25">
+        <v>6</v>
+      </c>
+      <c r="W25">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="26" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="O26">
+        <v>8</v>
+      </c>
+      <c r="Q26">
+        <v>60</v>
+      </c>
+      <c r="R26">
+        <v>64</v>
+      </c>
+      <c r="S26">
+        <f t="shared" si="0"/>
+        <v>124</v>
+      </c>
+      <c r="T26">
+        <f>U26-S26</f>
+        <v>650.31291699999997</v>
+      </c>
+      <c r="U26">
+        <v>774.31291699999997</v>
+      </c>
+      <c r="V26">
+        <v>10</v>
+      </c>
+      <c r="W26">
+        <f t="shared" si="1"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="27" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="O27">
+        <v>5</v>
+      </c>
+      <c r="Q27">
+        <v>62</v>
+      </c>
+      <c r="R27">
+        <v>64</v>
+      </c>
+      <c r="S27">
+        <f t="shared" si="0"/>
+        <v>126</v>
+      </c>
+      <c r="T27">
+        <f>U27-S27</f>
+        <v>507.665796</v>
+      </c>
+      <c r="U27">
+        <v>633.665796</v>
+      </c>
+      <c r="V27">
+        <v>20</v>
+      </c>
+      <c r="W27">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="28" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="O28">
         <v>4</v>
       </c>
-      <c r="I6" t="s">
+      <c r="Q28">
+        <v>62</v>
+      </c>
+      <c r="R28">
+        <v>63</v>
+      </c>
+      <c r="S28">
+        <f t="shared" si="0"/>
+        <v>125</v>
+      </c>
+      <c r="T28">
+        <f>U28-S28</f>
+        <v>481.68988400000001</v>
+      </c>
+      <c r="U28">
+        <v>606.68988400000001</v>
+      </c>
+      <c r="V28">
+        <v>30</v>
+      </c>
+      <c r="W28">
+        <f t="shared" si="1"/>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="29" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="O29">
+        <v>2</v>
+      </c>
+      <c r="Q29">
+        <v>60</v>
+      </c>
+      <c r="R29">
+        <v>63</v>
+      </c>
+      <c r="S29">
+        <f>Q29+R29</f>
+        <v>123</v>
+      </c>
+      <c r="T29">
+        <f>U29-S29</f>
+        <v>458.68473100000006</v>
+      </c>
+      <c r="U29">
+        <v>581.68473100000006</v>
+      </c>
+      <c r="V29">
+        <v>110</v>
+      </c>
+      <c r="W29">
+        <f>V29*O29*O29</f>
+        <v>440</v>
+      </c>
+    </row>
+    <row r="31" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="R31" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="Q33" t="s">
+        <v>9</v>
+      </c>
+      <c r="R33" t="s">
+        <v>5</v>
+      </c>
+      <c r="S33" t="s">
+        <v>10</v>
+      </c>
+      <c r="T33" t="s">
+        <v>11</v>
+      </c>
+      <c r="U33" t="s">
+        <v>15</v>
+      </c>
+      <c r="V33" t="s">
+        <v>16</v>
+      </c>
+      <c r="W33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="O34">
+        <v>16</v>
+      </c>
+      <c r="Q34">
+        <v>65</v>
+      </c>
+      <c r="R34">
+        <v>63</v>
+      </c>
+      <c r="S34">
+        <f t="shared" ref="S34:S38" si="3">Q34+R34</f>
+        <v>128</v>
+      </c>
+      <c r="T34">
+        <f>U34-S34</f>
+        <v>1272</v>
+      </c>
+      <c r="U34">
+        <v>1400</v>
+      </c>
+      <c r="V34">
+        <v>2.95</v>
+      </c>
+      <c r="W34">
+        <f t="shared" ref="W34:W38" si="4">V34*O34*O34</f>
+        <v>755.2</v>
+      </c>
+    </row>
+    <row r="35" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="O35">
+        <v>10</v>
+      </c>
+      <c r="Q35">
+        <v>64</v>
+      </c>
+      <c r="R35">
+        <v>63</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="3"/>
+        <v>127</v>
+      </c>
+      <c r="T35">
+        <f t="shared" ref="T35:T38" si="5">U35-S35</f>
+        <v>1053</v>
+      </c>
+      <c r="U35">
+        <v>1180</v>
+      </c>
+      <c r="V35">
+        <v>6.1</v>
+      </c>
+      <c r="W35">
+        <f t="shared" si="4"/>
+        <v>610</v>
+      </c>
+    </row>
+    <row r="36" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="O36">
+        <v>8</v>
+      </c>
+      <c r="Q36">
+        <v>60</v>
+      </c>
+      <c r="R36">
+        <v>64</v>
+      </c>
+      <c r="S36">
+        <f t="shared" si="3"/>
+        <v>124</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="5"/>
+        <v>646</v>
+      </c>
+      <c r="U36">
+        <v>770</v>
+      </c>
+      <c r="V36">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="W36">
+        <f t="shared" si="4"/>
+        <v>627.20000000000005</v>
+      </c>
+    </row>
+    <row r="37" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="O37">
+        <v>5</v>
+      </c>
+      <c r="Q37">
+        <v>62</v>
+      </c>
+      <c r="R37">
+        <v>64</v>
+      </c>
+      <c r="S37">
+        <f t="shared" si="3"/>
+        <v>126</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="5"/>
+        <v>499</v>
+      </c>
+      <c r="U37">
+        <v>625</v>
+      </c>
+      <c r="V37">
+        <v>20.5</v>
+      </c>
+      <c r="W37">
+        <f t="shared" si="4"/>
+        <v>512.5</v>
+      </c>
+    </row>
+    <row r="38" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="O38">
         <v>4</v>
       </c>
+      <c r="Q38">
+        <v>63</v>
+      </c>
+      <c r="R38">
+        <v>64</v>
+      </c>
+      <c r="S38">
+        <f t="shared" si="3"/>
+        <v>127</v>
+      </c>
+      <c r="T38">
+        <f t="shared" si="5"/>
+        <v>467.47930299999996</v>
+      </c>
+      <c r="U38">
+        <v>594.47930299999996</v>
+      </c>
+      <c r="V38">
+        <v>28.5</v>
+      </c>
+      <c r="W38">
+        <f t="shared" si="4"/>
+        <v>456</v>
+      </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F7">
-        <v>4</v>
-      </c>
-      <c r="G7">
-        <v>8</v>
-      </c>
-      <c r="H7">
-        <v>12</v>
-      </c>
-      <c r="I7">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F8">
-        <v>59.848300000000002</v>
-      </c>
-      <c r="G8">
-        <v>59.917299999999997</v>
-      </c>
-      <c r="H8">
-        <v>59.776200000000003</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" t="s">
-        <v>5</v>
-      </c>
-      <c r="G9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H9" t="s">
-        <v>5</v>
-      </c>
-      <c r="I9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F10">
-        <v>63.546495</v>
-      </c>
-      <c r="G10">
-        <v>63.262819</v>
-      </c>
-      <c r="H10">
-        <v>64.571686999999997</v>
+    <row r="39" spans="15:23" x14ac:dyDescent="0.25">
+      <c r="O39">
+        <v>2</v>
+      </c>
+      <c r="Q39">
+        <v>60</v>
+      </c>
+      <c r="R39">
+        <v>63</v>
+      </c>
+      <c r="S39">
+        <f>Q39+R39</f>
+        <v>123</v>
+      </c>
+      <c r="T39">
+        <f>U39-S39</f>
+        <v>440.16866600000003</v>
+      </c>
+      <c r="U39">
+        <v>563.16866600000003</v>
+      </c>
+      <c r="V39">
+        <v>108</v>
+      </c>
+      <c r="W39">
+        <f>V39*O39*O39</f>
+        <v>432</v>
       </c>
     </row>
   </sheetData>

</xml_diff>